<commit_message>
Added the xlsd library as it has the image scaling which is not in the released version of xlsxd.
</commit_message>
<xml_diff>
--- a/xlsxTest/x.xlsx
+++ b/xlsxTest/x.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -72,7 +72,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="itest_logo.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>